<commit_message>
feat : csv 파일 업로드
</commit_message>
<xml_diff>
--- a/DB_csv/교통사고예방시스템.xlsx
+++ b/DB_csv/교통사고예방시스템.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\29\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\29\Desktop\DB_Modeling_Project\DB_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23430" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23430" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="구 별 사고 정보" sheetId="3" r:id="rId2"/>
-    <sheet name="교통사고 발생현황" sheetId="2" r:id="rId3"/>
-    <sheet name="대전시 교통사고 정보" sheetId="4" r:id="rId4"/>
+    <sheet name="서구 사고 정보" sheetId="6" r:id="rId2"/>
+    <sheet name="중구 사고 정보" sheetId="7" r:id="rId3"/>
+    <sheet name="대덕구 사고정보" sheetId="8" r:id="rId4"/>
+    <sheet name="동구 사고 정보" sheetId="9" r:id="rId5"/>
+    <sheet name="유성구 사고 정보" sheetId="10" r:id="rId6"/>
+    <sheet name="교통사고 발생현황" sheetId="2" r:id="rId7"/>
+    <sheet name="대전시 교통사고 정보" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>사망</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,11 +141,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서구 사고 정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서구 사고 번호</t>
+    <t>과속 카메라 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테이블 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단속 테이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음주운전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신호위반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안전거리미확보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙선침범</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사고 건수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -149,7 +189,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>동이름</t>
+    <t>교통사고 날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교통사고 발생지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사상자 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 사고번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대전시 사고 관리 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -157,67 +217,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>과속 카메라 여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>음주 단속 여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테이블 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단속 테이블</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>음주운전</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신호위반</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과속</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안전거리미확보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중앙선침범</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사고 건수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대전시 사고 관리 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>교통사고 날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>교통사고 발생지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사상자 수</t>
+    <t>음주단속 여부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -406,37 +406,37 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -958,34 +958,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -1016,35 +1016,35 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
@@ -1054,40 +1054,40 @@
       <c r="F14" s="1"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="15"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="17"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
@@ -1140,22 +1140,22 @@
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1166,117 +1166,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B26"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>33</v>
+      <c r="F1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1287,9 +1210,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1309,32 +1284,32 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1361,16 +1336,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>